<commit_message>
import multi sheet initialized
</commit_message>
<xml_diff>
--- a/de.bund.bfr.knime.openkrise.db/src/org/hsh/bfr/db/imports/custom/bfrnewformat/BfR_Format_Backtrace_multi.xlsx
+++ b/de.bund.bfr.knime.openkrise.db/src/org/hsh/bfr/db/imports/custom/bfrnewformat/BfR_Format_Backtrace_multi.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="124">
   <si>
     <t>Product Number</t>
   </si>
@@ -740,7 +740,55 @@
     <xf numFmtId="49" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -763,6 +811,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="11" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -770,6 +825,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -777,62 +833,6 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal 2" xfId="2"/>
@@ -1138,44 +1138,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="85.5703125" customWidth="1"/>
     <col min="2" max="2" width="49.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="55"/>
+    <col min="3" max="3" width="11.42578125" style="35"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C2" s="54"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1184,15 +1182,15 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>OutgoingDeliveries!$I:$I</xm:f>
+            <xm:f>Lot!$O:$O</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A1048576</xm:sqref>
+          <xm:sqref>B2:B1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Lot!$O:$O</xm:f>
+            <xm:f>OutgoingDeliveries!$K:$K</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B1048576</xm:sqref>
+          <xm:sqref>A2:A1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1223,61 +1221,61 @@
     <col min="13" max="13" width="21" style="2" customWidth="1"/>
     <col min="14" max="14" width="17.140625" style="2" customWidth="1"/>
     <col min="15" max="15" width="17.85546875" style="2" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" style="50"/>
+    <col min="16" max="16" width="9.140625" style="31"/>
     <col min="17" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="32" t="s">
+      <c r="F1" s="46"/>
+      <c r="G1" s="47" t="s">
         <v>119</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="32" t="s">
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="47" t="s">
         <v>120</v>
       </c>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="32" t="s">
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="47" t="s">
         <v>121</v>
       </c>
-      <c r="N1" s="33" t="s">
+      <c r="N1" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="O1" s="45" t="s">
+      <c r="O1" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="P1" s="38" t="s">
+      <c r="P1" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
-      <c r="T1" s="39"/>
-      <c r="U1" s="39"/>
-      <c r="V1" s="39"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
     </row>
     <row r="2" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
+      <c r="A2" s="44"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
       <c r="E2" s="21" t="s">
         <v>116</v>
       </c>
@@ -1302,16 +1300,16 @@
       <c r="L2" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="39"/>
-      <c r="V2" s="39"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="40"/>
+      <c r="V2" s="40"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="O3" s="2" t="str">
@@ -1597,11 +1595,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="T1:T2"/>
     <mergeCell ref="U1:U2"/>
     <mergeCell ref="V1:V2"/>
     <mergeCell ref="O1:O2"/>
@@ -1614,6 +1607,11 @@
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="M1:M2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="T1:T2"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E1048576">
@@ -1669,10 +1667,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S40"/>
+  <dimension ref="A1:R40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1686,52 +1684,49 @@
     <col min="7" max="7" width="16.85546875" style="2" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" style="2"/>
     <col min="9" max="9" width="30.28515625" style="2" customWidth="1"/>
-    <col min="10" max="12" width="11.42578125" style="2"/>
-    <col min="13" max="13" width="11.42578125" style="50"/>
-    <col min="14" max="14" width="11.42578125" style="2"/>
-    <col min="15" max="15" width="14.5703125" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="11.42578125" style="2"/>
+    <col min="10" max="11" width="11.42578125" style="2"/>
+    <col min="12" max="12" width="11.42578125" style="31"/>
+    <col min="13" max="13" width="11.42578125" style="2"/>
+    <col min="14" max="14" width="14.5703125" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:18" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="54" t="s">
         <v>111</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="34" t="s">
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="36" t="s">
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="I1" s="37"/>
-      <c r="J1" s="34" t="s">
+      <c r="I1" s="55"/>
+      <c r="J1" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="34" t="s">
-        <v>110</v>
-      </c>
-      <c r="L1" s="45" t="s">
+      <c r="K1" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="M1" s="49" t="s">
+      <c r="L1" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="N1" s="47"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="53"/>
       <c r="B2" s="19" t="s">
         <v>113</v>
       </c>
@@ -1756,375 +1751,373 @@
       <c r="I2" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J2" s="52"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L3" s="2" t="str">
+      <c r="K3" s="2" t="str">
         <f>A3&amp;","&amp;C3&amp;"."&amp;D3&amp;"."&amp;E3&amp;J3</f>
         <v xml:space="preserve"> , ,..</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L4" s="2" t="str">
-        <f t="shared" ref="L4:L40" si="0">A4&amp;","&amp;C4&amp;"."&amp;D4&amp;"."&amp;E4&amp;J4</f>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K4" s="2" t="str">
+        <f t="shared" ref="K4:K40" si="0">A4&amp;","&amp;C4&amp;"."&amp;D4&amp;"."&amp;E4&amp;J4</f>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L5" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L6" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L7" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L8" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L9" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L11" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L12" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L13" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L14" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L15" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K15" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L16" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L17" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L18" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L19" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K19" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L20" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L21" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K21" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L22" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K22" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L23" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K23" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L24" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K24" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L25" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K25" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L26" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K26" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L27" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K27" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L28" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K28" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L29" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K29" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L30" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K30" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L31" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K31" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L32" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K32" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L33" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K33" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L34" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K34" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L35" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K35" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L36" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K36" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L37" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K37" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L38" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K38" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L39" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> , ,..</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K39" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> , ,..</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="L40" s="2" t="str">
+      <c r="K40" s="2" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> , ,..</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="13">
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:I1"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G1048576 D3:D1048576">
@@ -2142,7 +2135,7 @@
     <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:L2 T1:XFD2"/>
+    <dataValidation operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S1:XFD2 A1:K2"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2177,7 +2170,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>